<commit_message>
Added Sentinel-2 NG band pass info
Updates from VHRODA 2024 presentation
</commit_message>
<xml_diff>
--- a/data/sentinel2ng/sentinel2ng.xlsx
+++ b/data/sentinel2ng/sentinel2ng.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\PycharmProjects\datacube.spectral\data\sentinel2ng\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53ACEBA-A336-4D2B-B647-719FD525B800}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D17078C-7E2B-41A6-A268-8EC64D32F6BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27510" yWindow="2505" windowWidth="21600" windowHeight="11295" xr2:uid="{B7065FAE-5E99-4DC8-B44A-6ECDF5205C1D}"/>
+    <workbookView xWindow="0" yWindow="1065" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{B7065FAE-5E99-4DC8-B44A-6ECDF5205C1D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="lplanet2022" sheetId="1" r:id="rId1"/>
+    <sheet name="vhroda2024" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="59">
   <si>
     <t>SSD Goal</t>
   </si>
@@ -156,16 +157,81 @@
   </si>
   <si>
     <t>Bandwidth</t>
+  </si>
+  <si>
+    <t>Lref</t>
+  </si>
+  <si>
+    <t>SNR</t>
+  </si>
+  <si>
+    <t>1(H)</t>
+  </si>
+  <si>
+    <t>2(H)</t>
+  </si>
+  <si>
+    <t>4(H)</t>
+  </si>
+  <si>
+    <t>5(H)</t>
+  </si>
+  <si>
+    <t>6(H)</t>
+  </si>
+  <si>
+    <t>7(H)</t>
+  </si>
+  <si>
+    <t>8(H)</t>
+  </si>
+  <si>
+    <t>8a(H)</t>
+  </si>
+  <si>
+    <t>9(H)</t>
+  </si>
+  <si>
+    <t>10(H)</t>
+  </si>
+  <si>
+    <t>11(H)</t>
+  </si>
+  <si>
+    <t>3(H)</t>
+  </si>
+  <si>
+    <t>current[m]</t>
+  </si>
+  <si>
+    <t>SSD[m]</t>
+  </si>
+  <si>
+    <t>CWvl[nm]</t>
+  </si>
+  <si>
+    <t>BW[nm]</t>
+  </si>
+  <si>
+    <t>https://earth.esa.int/eogateway/documents/d/earth-online/15_sproud_esa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -188,13 +254,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -529,8 +598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5286E426-19FD-4306-BA1E-1B27ACFFE889}">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1115,4 +1184,512 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E3F5B09-3724-4EFF-BDFD-84E63D41A14D}">
+  <dimension ref="A1:G23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+      <c r="D3">
+        <v>412</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>45</v>
+      </c>
+      <c r="G3">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4">
+        <v>60</v>
+      </c>
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>443</v>
+      </c>
+      <c r="E4">
+        <v>20</v>
+      </c>
+      <c r="F4">
+        <v>129.11000000000001</v>
+      </c>
+      <c r="G4">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>475</v>
+      </c>
+      <c r="E5">
+        <v>20</v>
+      </c>
+      <c r="F5">
+        <v>90.7</v>
+      </c>
+      <c r="G5">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>490</v>
+      </c>
+      <c r="E6">
+        <v>65</v>
+      </c>
+      <c r="F6">
+        <v>128</v>
+      </c>
+      <c r="G6">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <v>520</v>
+      </c>
+      <c r="E7">
+        <v>15</v>
+      </c>
+      <c r="F7">
+        <v>80.5</v>
+      </c>
+      <c r="G7">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>560</v>
+      </c>
+      <c r="E8">
+        <v>35</v>
+      </c>
+      <c r="F8">
+        <v>128</v>
+      </c>
+      <c r="G8">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <v>620</v>
+      </c>
+      <c r="E9">
+        <v>30</v>
+      </c>
+      <c r="F9">
+        <v>29.8</v>
+      </c>
+      <c r="G9">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>20</v>
+      </c>
+      <c r="D10">
+        <v>650</v>
+      </c>
+      <c r="E10">
+        <v>20</v>
+      </c>
+      <c r="F10">
+        <v>29.8</v>
+      </c>
+      <c r="G10">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>665</v>
+      </c>
+      <c r="E11">
+        <v>30</v>
+      </c>
+      <c r="F11">
+        <v>108</v>
+      </c>
+      <c r="G11">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12">
+        <v>20</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>705</v>
+      </c>
+      <c r="E12">
+        <v>15</v>
+      </c>
+      <c r="F12">
+        <v>74.599999999999994</v>
+      </c>
+      <c r="G12">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13">
+        <v>20</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <v>740</v>
+      </c>
+      <c r="E13">
+        <v>15</v>
+      </c>
+      <c r="F13">
+        <v>68.23</v>
+      </c>
+      <c r="G13">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14">
+        <v>20</v>
+      </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>783</v>
+      </c>
+      <c r="E14">
+        <v>20</v>
+      </c>
+      <c r="F14">
+        <v>66.7</v>
+      </c>
+      <c r="G14">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>842</v>
+      </c>
+      <c r="E15">
+        <v>115</v>
+      </c>
+      <c r="F15">
+        <v>103</v>
+      </c>
+      <c r="G15">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16">
+        <v>20</v>
+      </c>
+      <c r="C16">
+        <v>10</v>
+      </c>
+      <c r="D16">
+        <v>865</v>
+      </c>
+      <c r="E16">
+        <v>20</v>
+      </c>
+      <c r="F16">
+        <v>52.39</v>
+      </c>
+      <c r="G16">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17">
+        <v>60</v>
+      </c>
+      <c r="C17">
+        <v>60</v>
+      </c>
+      <c r="D17">
+        <v>945</v>
+      </c>
+      <c r="E17">
+        <v>20</v>
+      </c>
+      <c r="F17">
+        <v>8.77</v>
+      </c>
+      <c r="G17">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18">
+        <v>60</v>
+      </c>
+      <c r="D18">
+        <v>985</v>
+      </c>
+      <c r="E18">
+        <v>20</v>
+      </c>
+      <c r="F18">
+        <v>56.4</v>
+      </c>
+      <c r="G18">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19">
+        <v>60</v>
+      </c>
+      <c r="C19">
+        <v>60</v>
+      </c>
+      <c r="D19">
+        <v>1375</v>
+      </c>
+      <c r="E19">
+        <v>30</v>
+      </c>
+      <c r="F19">
+        <v>6</v>
+      </c>
+      <c r="G19">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20">
+        <v>20</v>
+      </c>
+      <c r="C20">
+        <v>10</v>
+      </c>
+      <c r="D20">
+        <v>1610</v>
+      </c>
+      <c r="E20">
+        <v>90</v>
+      </c>
+      <c r="F20">
+        <v>4</v>
+      </c>
+      <c r="G20">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <v>10</v>
+      </c>
+      <c r="D21">
+        <v>2130</v>
+      </c>
+      <c r="E21">
+        <v>50</v>
+      </c>
+      <c r="F21">
+        <v>1.7</v>
+      </c>
+      <c r="G21">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22">
+        <v>20</v>
+      </c>
+      <c r="C22">
+        <v>10</v>
+      </c>
+      <c r="D22">
+        <v>2210</v>
+      </c>
+      <c r="E22">
+        <v>50</v>
+      </c>
+      <c r="F22">
+        <v>1.7</v>
+      </c>
+      <c r="G22">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23">
+        <v>20</v>
+      </c>
+      <c r="C23">
+        <v>10</v>
+      </c>
+      <c r="D23">
+        <v>2260</v>
+      </c>
+      <c r="E23">
+        <v>50</v>
+      </c>
+      <c r="F23">
+        <v>1.7</v>
+      </c>
+      <c r="G23">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>